<commit_message>
reorganize repository DOH data drop for 20210526
</commit_message>
<xml_diff>
--- a/misc/peter/COVID-Model.xlsx
+++ b/misc/peter/COVID-Model.xlsx
@@ -294,11 +294,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1818499260"/>
-        <c:axId val="1390834969"/>
+        <c:axId val="1734404425"/>
+        <c:axId val="616675659"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1818499260"/>
+        <c:axId val="1734404425"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,10 +350,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1390834969"/>
+        <c:crossAx val="616675659"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1390834969"/>
+        <c:axId val="616675659"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,7 +428,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1818499260"/>
+        <c:crossAx val="1734404425"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -515,11 +515,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="140685541"/>
-        <c:axId val="795832144"/>
+        <c:axId val="1621047025"/>
+        <c:axId val="619131225"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140685541"/>
+        <c:axId val="1621047025"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,10 +571,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="795832144"/>
+        <c:crossAx val="619131225"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="795832144"/>
+        <c:axId val="619131225"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -649,7 +649,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140685541"/>
+        <c:crossAx val="1621047025"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -741,11 +741,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="855659764"/>
-        <c:axId val="1654799327"/>
+        <c:axId val="1910190459"/>
+        <c:axId val="1464870050"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="855659764"/>
+        <c:axId val="1910190459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,10 +797,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1654799327"/>
+        <c:crossAx val="1464870050"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1654799327"/>
+        <c:axId val="1464870050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -875,7 +875,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="855659764"/>
+        <c:crossAx val="1910190459"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -980,11 +980,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="460992148"/>
-        <c:axId val="2019549197"/>
+        <c:axId val="1437653342"/>
+        <c:axId val="1879624580"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="460992148"/>
+        <c:axId val="1437653342"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,10 +1036,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2019549197"/>
+        <c:crossAx val="1879624580"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2019549197"/>
+        <c:axId val="1879624580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1114,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="460992148"/>
+        <c:crossAx val="1437653342"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1206,11 +1206,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="914976255"/>
-        <c:axId val="74069339"/>
+        <c:axId val="1009623047"/>
+        <c:axId val="1610778305"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="914976255"/>
+        <c:axId val="1009623047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,10 +1262,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74069339"/>
+        <c:crossAx val="1610778305"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74069339"/>
+        <c:axId val="1610778305"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1340,7 +1340,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="914976255"/>
+        <c:crossAx val="1009623047"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1432,11 +1432,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2112002150"/>
-        <c:axId val="2031830898"/>
+        <c:axId val="893303339"/>
+        <c:axId val="307604935"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2112002150"/>
+        <c:axId val="893303339"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,10 +1488,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2031830898"/>
+        <c:crossAx val="307604935"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2031830898"/>
+        <c:axId val="307604935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,7 +1566,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112002150"/>
+        <c:crossAx val="893303339"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1719,11 +1719,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="107009292"/>
-        <c:axId val="264748431"/>
+        <c:axId val="1952527966"/>
+        <c:axId val="2085180958"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107009292"/>
+        <c:axId val="1952527966"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,10 +1775,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264748431"/>
+        <c:crossAx val="2085180958"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="264748431"/>
+        <c:axId val="2085180958"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1853,7 +1853,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107009292"/>
+        <c:crossAx val="1952527966"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1947,11 +1947,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1041162834"/>
-        <c:axId val="349148115"/>
+        <c:axId val="1903730320"/>
+        <c:axId val="596196226"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1041162834"/>
+        <c:axId val="1903730320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,10 +2003,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349148115"/>
+        <c:crossAx val="596196226"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349148115"/>
+        <c:axId val="596196226"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2081,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1041162834"/>
+        <c:crossAx val="1903730320"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>